<commit_message>
correct exp1 images name
</commit_message>
<xml_diff>
--- a/exp1_best_parameters.xlsx
+++ b/exp1_best_parameters.xlsx
@@ -31,18 +31,21 @@
     <t>Clip_Limit</t>
   </si>
   <si>
+    <t>D0.jpg</t>
+  </si>
+  <si>
+    <t>GHE</t>
+  </si>
+  <si>
+    <t>AHE</t>
+  </si>
+  <si>
+    <t>CLAHE</t>
+  </si>
+  <si>
     <t>D1.jpg</t>
   </si>
   <si>
-    <t>GHE</t>
-  </si>
-  <si>
-    <t>AHE</t>
-  </si>
-  <si>
-    <t>CLAHE</t>
-  </si>
-  <si>
     <t>D2.jpg</t>
   </si>
   <si>
@@ -52,7 +55,7 @@
     <t>D4.jpg</t>
   </si>
   <si>
-    <t>D5.jpg</t>
+    <t>L0.jpg</t>
   </si>
   <si>
     <t>L1.jpg</t>
@@ -65,9 +68,6 @@
   </si>
   <si>
     <t>L4.jpg</t>
-  </si>
-  <si>
-    <t>L5.jpg</t>
   </si>
 </sst>
 </file>
@@ -1215,7 +1215,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="A1:H11"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="7"/>

</xml_diff>